<commit_message>
bai try catch debug
</commit_message>
<xml_diff>
--- a/[BC-JAVA-APJ] Advanced Programming with Java v2.0_C1222I1.xlsx
+++ b/[BC-JAVA-APJ] Advanced Programming with Java v2.0_C1222I1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODEGYM\CODEGYM\Module2\C1222I1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9155C749-8C12-4F74-9943-6EDCFF2AD7C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B14DDD-FDC1-4649-AEBE-EA4B2986F210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2376,6 +2376,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2392,7 +2393,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2728,8 +2728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I22" sqref="A17:I22"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2929,10 +2929,10 @@
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
@@ -2965,10 +2965,10 @@
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="122"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
@@ -4397,16 +4397,16 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D39" s="123" t="s">
+      <c r="D39" s="124" t="s">
         <v>115</v>
       </c>
-      <c r="E39" s="124"/>
-      <c r="F39" s="125"/>
-      <c r="G39" s="126" t="s">
+      <c r="E39" s="125"/>
+      <c r="F39" s="126"/>
+      <c r="G39" s="127" t="s">
         <v>116</v>
       </c>
-      <c r="H39" s="124"/>
-      <c r="I39" s="125"/>
+      <c r="H39" s="125"/>
+      <c r="I39" s="126"/>
       <c r="J39" s="28"/>
       <c r="K39" s="1"/>
       <c r="M39" s="1"/>
@@ -4436,14 +4436,14 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D40" s="127" t="s">
+      <c r="D40" s="128" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="124"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="124"/>
-      <c r="H40" s="124"/>
-      <c r="I40" s="125"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="125"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="125"/>
+      <c r="I40" s="126"/>
       <c r="J40" s="31" t="s">
         <v>119</v>
       </c>
@@ -12426,10 +12426,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C3019F-F7BC-4143-A419-C938F37317BB}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12437,20 +12437,24 @@
     <col min="1" max="1" width="11.28515625" style="118" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
         <v>450</v>
       </c>
-      <c r="B1" s="129">
+      <c r="B1" s="121">
         <v>44973</v>
       </c>
-      <c r="C1" s="129">
+      <c r="C1" s="121">
         <v>44974</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="121">
+        <v>44977</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="118" t="s">
         <v>451</v>
       </c>
@@ -12460,8 +12464,11 @@
       <c r="C2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="118" t="s">
         <v>452</v>
       </c>
@@ -12471,8 +12478,11 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="118" t="s">
         <v>453</v>
       </c>
@@ -12482,8 +12492,11 @@
       <c r="C4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="118" t="s">
         <v>454</v>
       </c>
@@ -12493,8 +12506,11 @@
       <c r="C5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="118" t="s">
         <v>455</v>
       </c>
@@ -12503,6 +12519,9 @@
       </c>
       <c r="C6">
         <v>0</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -12639,10 +12658,10 @@
       <c r="A7" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="129" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="55" t="s">
         <v>146</v>
       </c>
@@ -12668,10 +12687,10 @@
       <c r="A8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="129" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="122"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="55" t="s">
         <v>151</v>
       </c>
@@ -12697,10 +12716,10 @@
       <c r="A9" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="129" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="122"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="2"/>
       <c r="E9" s="11" t="s">
         <v>157</v>
@@ -12724,10 +12743,10 @@
       <c r="A10" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="128" t="s">
+      <c r="B10" s="129" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="122"/>
+      <c r="C10" s="123"/>
       <c r="D10" s="55" t="s">
         <v>18</v>
       </c>
@@ -21058,10 +21077,10 @@
       <c r="A6" s="55" t="s">
         <v>420</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="129" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="122"/>
+      <c r="C6" s="123"/>
       <c r="D6" s="55" t="s">
         <v>146</v>
       </c>
@@ -21085,10 +21104,10 @@
       <c r="A7" s="55" t="s">
         <v>423</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="129" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="55" t="s">
         <v>151</v>
       </c>
@@ -21111,10 +21130,10 @@
       <c r="A8" s="55" t="s">
         <v>427</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="129" t="s">
         <v>428</v>
       </c>
-      <c r="C8" s="122"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="55" t="s">
         <v>18</v>
       </c>

</xml_diff>